<commit_message>
feat: add actioning airdrop
</commit_message>
<xml_diff>
--- a/RClick/Assets.xcassets/template.dataset/template.xlsx
+++ b/RClick/Assets.xcassets/template.dataset/template.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
@@ -914,6 +914,13 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1166,26 +1173,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="2"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>2</v>
-      </c>
-      <c r="C1">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>